<commit_message>
Vicon data QDM calcul
Calculation onf QDM with VICON Data, i use gitignore to not commit full data but the file xlsx final is here.
</commit_message>
<xml_diff>
--- a/results/vicon_QDM_wrists_head_mm.xlsx
+++ b/results/vicon_QDM_wrists_head_mm.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:V37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,7 +548,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/test/VICON_CSV/SEATEDD01.csv</t>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEATEDD01.csv</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -620,145 +620,2521 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/test/VICON_CSV/SEMID01.csv</t>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEATEDD02.csv</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SEMID01.csv</t>
+          <t>SEATEDD02.csv</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>8668.166076665064</v>
+        <v>15422.89401213957</v>
       </c>
       <c r="D3" t="n">
         <v>17999</v>
       </c>
       <c r="E3" t="n">
-        <v>6035.964257009496</v>
+        <v>16779.29237335427</v>
       </c>
       <c r="F3" t="n">
         <v>17999</v>
       </c>
       <c r="G3" t="n">
-        <v>14704.13033367456</v>
+        <v>32202.18638549384</v>
       </c>
       <c r="H3" t="n">
-        <v>13942.42811964512</v>
+        <v>9725.644868964118</v>
       </c>
       <c r="I3" t="n">
         <v>17999</v>
       </c>
       <c r="J3" t="n">
-        <v>14935.84173361575</v>
+        <v>10354.21281121635</v>
       </c>
       <c r="K3" t="n">
         <v>17999</v>
       </c>
       <c r="L3" t="n">
-        <v>28878.26985326087</v>
+        <v>20079.85768018047</v>
       </c>
       <c r="M3" t="n">
-        <v>7473.133557300522</v>
+        <v>16420.18908564422</v>
       </c>
       <c r="N3" t="n">
         <v>17999</v>
       </c>
       <c r="O3" t="n">
-        <v>8656.559834993594</v>
+        <v>17622.88955704405</v>
       </c>
       <c r="P3" t="n">
         <v>17999</v>
       </c>
       <c r="Q3" t="n">
-        <v>16129.69339229412</v>
+        <v>34043.07864268827</v>
       </c>
       <c r="R3" t="n">
-        <v>8852.532002180582</v>
+        <v>9851.813432939904</v>
       </c>
       <c r="S3" t="n">
         <v>17999</v>
       </c>
       <c r="T3" t="n">
-        <v>9113.59736809379</v>
+        <v>10217.11878169352</v>
       </c>
       <c r="U3" t="n">
         <v>17999</v>
       </c>
       <c r="V3" t="n">
-        <v>17966.12937027437</v>
+        <v>20068.93221463342</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/test/VICON_CSV/STANDINGD01.csv</t>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEATEDD03.csv</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>SEATEDD03.csv</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>34870.99226695849</v>
+      </c>
+      <c r="D4" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E4" t="n">
+        <v>27170.83167788099</v>
+      </c>
+      <c r="F4" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G4" t="n">
+        <v>62041.82394483948</v>
+      </c>
+      <c r="H4" t="n">
+        <v>14105.98014792927</v>
+      </c>
+      <c r="I4" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J4" t="n">
+        <v>14473.34665148227</v>
+      </c>
+      <c r="K4" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L4" t="n">
+        <v>28579.32679941154</v>
+      </c>
+      <c r="M4" t="n">
+        <v>19508.82754992634</v>
+      </c>
+      <c r="N4" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O4" t="n">
+        <v>6708.991776539241</v>
+      </c>
+      <c r="P4" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>26217.81932646558</v>
+      </c>
+      <c r="R4" t="n">
+        <v>8916.973687164789</v>
+      </c>
+      <c r="S4" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T4" t="n">
+        <v>9655.490832541203</v>
+      </c>
+      <c r="U4" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V4" t="n">
+        <v>18572.46451970599</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEATEDD04.csv</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SEATEDD04.csv</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2661.923273848382</v>
+      </c>
+      <c r="D5" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3833.346975659305</v>
+      </c>
+      <c r="F5" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G5" t="n">
+        <v>6495.270249507687</v>
+      </c>
+      <c r="H5" t="n">
+        <v>4847.753224850871</v>
+      </c>
+      <c r="I5" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J5" t="n">
+        <v>4768.206438907198</v>
+      </c>
+      <c r="K5" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L5" t="n">
+        <v>9615.959663758069</v>
+      </c>
+      <c r="M5" t="n">
+        <v>7680.839057542305</v>
+      </c>
+      <c r="N5" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O5" t="n">
+        <v>11250.40228143005</v>
+      </c>
+      <c r="P5" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>18931.24133897236</v>
+      </c>
+      <c r="R5" t="n">
+        <v>7442.981553029516</v>
+      </c>
+      <c r="S5" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T5" t="n">
+        <v>7080.281922950293</v>
+      </c>
+      <c r="U5" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V5" t="n">
+        <v>14523.26347597981</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEATEDD05.csv</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SEATEDD05.csv</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>6273.53842874073</v>
+      </c>
+      <c r="D6" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E6" t="n">
+        <v>6588.36258583828</v>
+      </c>
+      <c r="F6" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G6" t="n">
+        <v>12861.90101457901</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4558.721873818168</v>
+      </c>
+      <c r="I6" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J6" t="n">
+        <v>4829.197593008849</v>
+      </c>
+      <c r="K6" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L6" t="n">
+        <v>9387.919466827017</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2684.09941089313</v>
+      </c>
+      <c r="N6" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O6" t="n">
+        <v>5080.767751223239</v>
+      </c>
+      <c r="P6" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>7764.867162116368</v>
+      </c>
+      <c r="R6" t="n">
+        <v>5805.341912693714</v>
+      </c>
+      <c r="S6" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T6" t="n">
+        <v>5511.189012280902</v>
+      </c>
+      <c r="U6" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V6" t="n">
+        <v>11316.53092497462</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEATEDD06.csv</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SEATEDD06.csv</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>11482.06125073784</v>
+      </c>
+      <c r="D7" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E7" t="n">
+        <v>13070.76307033855</v>
+      </c>
+      <c r="F7" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G7" t="n">
+        <v>24552.82432107639</v>
+      </c>
+      <c r="H7" t="n">
+        <v>10500.14773574605</v>
+      </c>
+      <c r="I7" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J7" t="n">
+        <v>10877.22453551572</v>
+      </c>
+      <c r="K7" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L7" t="n">
+        <v>21377.37227126177</v>
+      </c>
+      <c r="M7" t="n">
+        <v>9728.614497955052</v>
+      </c>
+      <c r="N7" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O7" t="n">
+        <v>10180.77677885512</v>
+      </c>
+      <c r="P7" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>19909.39127681017</v>
+      </c>
+      <c r="R7" t="n">
+        <v>10419.49761150055</v>
+      </c>
+      <c r="S7" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T7" t="n">
+        <v>10772.15671707018</v>
+      </c>
+      <c r="U7" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V7" t="n">
+        <v>21191.65432857074</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEATEDD07.csv</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SEATEDD07.csv</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>9802.537101863409</v>
+      </c>
+      <c r="D8" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E8" t="n">
+        <v>8134.376382197508</v>
+      </c>
+      <c r="F8" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G8" t="n">
+        <v>17936.91348406092</v>
+      </c>
+      <c r="H8" t="n">
+        <v>5884.760235871346</v>
+      </c>
+      <c r="I8" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J8" t="n">
+        <v>6170.684144347587</v>
+      </c>
+      <c r="K8" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L8" t="n">
+        <v>12055.44438021893</v>
+      </c>
+      <c r="M8" t="n">
+        <v>12555.4370304069</v>
+      </c>
+      <c r="N8" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O8" t="n">
+        <v>13529.55075726701</v>
+      </c>
+      <c r="P8" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>26084.98778767391</v>
+      </c>
+      <c r="R8" t="n">
+        <v>8263.415484837886</v>
+      </c>
+      <c r="S8" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T8" t="n">
+        <v>7838.102261773041</v>
+      </c>
+      <c r="U8" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V8" t="n">
+        <v>16101.51774661093</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEATEDD08.csv</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SEATEDD08.csv</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>12391.59599663952</v>
+      </c>
+      <c r="D9" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E9" t="n">
+        <v>7032.863643195496</v>
+      </c>
+      <c r="F9" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G9" t="n">
+        <v>19424.45963983501</v>
+      </c>
+      <c r="H9" t="n">
+        <v>8247.951476681654</v>
+      </c>
+      <c r="I9" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J9" t="n">
+        <v>7904.140424515247</v>
+      </c>
+      <c r="K9" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L9" t="n">
+        <v>16152.0919011969</v>
+      </c>
+      <c r="M9" t="n">
+        <v>10612.73232351746</v>
+      </c>
+      <c r="N9" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O9" t="n">
+        <v>19406.99964315136</v>
+      </c>
+      <c r="P9" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>30019.73196666882</v>
+      </c>
+      <c r="R9" t="n">
+        <v>10175.95648137923</v>
+      </c>
+      <c r="S9" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T9" t="n">
+        <v>9455.445587950535</v>
+      </c>
+      <c r="U9" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V9" t="n">
+        <v>19631.40206932976</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEATEDD09.csv</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SEATEDD09.csv</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>15671.89921960912</v>
+      </c>
+      <c r="D10" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E10" t="n">
+        <v>9542.586048437892</v>
+      </c>
+      <c r="F10" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G10" t="n">
+        <v>25214.48526804701</v>
+      </c>
+      <c r="H10" t="n">
+        <v>7377.101123171716</v>
+      </c>
+      <c r="I10" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J10" t="n">
+        <v>7088.189469542334</v>
+      </c>
+      <c r="K10" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L10" t="n">
+        <v>14465.29059271405</v>
+      </c>
+      <c r="M10" t="n">
+        <v>8268.239263995492</v>
+      </c>
+      <c r="N10" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O10" t="n">
+        <v>13727.91540784088</v>
+      </c>
+      <c r="P10" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>21996.15467183638</v>
+      </c>
+      <c r="R10" t="n">
+        <v>6997.089279223671</v>
+      </c>
+      <c r="S10" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T10" t="n">
+        <v>7607.390885771348</v>
+      </c>
+      <c r="U10" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V10" t="n">
+        <v>14604.48016499502</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEATEDD10.csv</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SEATEDD10.csv</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2988.110842658282</v>
+      </c>
+      <c r="D11" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2707.346798527488</v>
+      </c>
+      <c r="F11" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G11" t="n">
+        <v>5695.457641185771</v>
+      </c>
+      <c r="H11" t="n">
+        <v>5239.616492807777</v>
+      </c>
+      <c r="I11" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J11" t="n">
+        <v>5215.8890656015</v>
+      </c>
+      <c r="K11" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L11" t="n">
+        <v>10455.50555840928</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1531.093917842078</v>
+      </c>
+      <c r="N11" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1880.642967018161</v>
+      </c>
+      <c r="P11" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>3411.736884860239</v>
+      </c>
+      <c r="R11" t="n">
+        <v>4876.40693825623</v>
+      </c>
+      <c r="S11" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T11" t="n">
+        <v>5215.268807103054</v>
+      </c>
+      <c r="U11" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V11" t="n">
+        <v>10091.67574535928</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEATEDD11.csv</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SEATEDD11.csv</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>11755.57071966501</v>
+      </c>
+      <c r="D12" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6013.679873587428</v>
+      </c>
+      <c r="F12" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G12" t="n">
+        <v>17769.25059325244</v>
+      </c>
+      <c r="H12" t="n">
+        <v>8062.33969574448</v>
+      </c>
+      <c r="I12" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J12" t="n">
+        <v>8162.899527903734</v>
+      </c>
+      <c r="K12" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L12" t="n">
+        <v>16225.23922364822</v>
+      </c>
+      <c r="M12" t="n">
+        <v>7236.521559165006</v>
+      </c>
+      <c r="N12" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O12" t="n">
+        <v>6465.647014535556</v>
+      </c>
+      <c r="P12" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>13702.16857370056</v>
+      </c>
+      <c r="R12" t="n">
+        <v>5914.206388197624</v>
+      </c>
+      <c r="S12" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T12" t="n">
+        <v>5627.339838358163</v>
+      </c>
+      <c r="U12" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V12" t="n">
+        <v>11541.54622655579</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEATEDD12.csv</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SEATEDD12.csv</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>44429.5062947374</v>
+      </c>
+      <c r="D13" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E13" t="n">
+        <v>45290.39094908789</v>
+      </c>
+      <c r="F13" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G13" t="n">
+        <v>89719.89724382528</v>
+      </c>
+      <c r="H13" t="n">
+        <v>11906.30596055814</v>
+      </c>
+      <c r="I13" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J13" t="n">
+        <v>12645.7161419169</v>
+      </c>
+      <c r="K13" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L13" t="n">
+        <v>24552.02210247504</v>
+      </c>
+      <c r="M13" t="n">
+        <v>12907.81168585761</v>
+      </c>
+      <c r="N13" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O13" t="n">
+        <v>11278.59905250692</v>
+      </c>
+      <c r="P13" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>24186.41073836453</v>
+      </c>
+      <c r="R13" t="n">
+        <v>7528.875386132569</v>
+      </c>
+      <c r="S13" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T13" t="n">
+        <v>6308.960799299228</v>
+      </c>
+      <c r="U13" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V13" t="n">
+        <v>13837.8361854318</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEMID01.csv</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SEMID01.csv</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>8668.166076665064</v>
+      </c>
+      <c r="D14" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E14" t="n">
+        <v>6035.964257009496</v>
+      </c>
+      <c r="F14" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G14" t="n">
+        <v>14704.13033367456</v>
+      </c>
+      <c r="H14" t="n">
+        <v>13942.42811964512</v>
+      </c>
+      <c r="I14" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J14" t="n">
+        <v>14935.84173361575</v>
+      </c>
+      <c r="K14" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L14" t="n">
+        <v>28878.26985326087</v>
+      </c>
+      <c r="M14" t="n">
+        <v>7473.133557300522</v>
+      </c>
+      <c r="N14" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O14" t="n">
+        <v>8656.559834993594</v>
+      </c>
+      <c r="P14" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>16129.69339229412</v>
+      </c>
+      <c r="R14" t="n">
+        <v>8852.532002180582</v>
+      </c>
+      <c r="S14" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T14" t="n">
+        <v>9113.59736809379</v>
+      </c>
+      <c r="U14" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V14" t="n">
+        <v>17966.12937027437</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEMID02.csv</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SEMID02.csv</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>11816.04235853448</v>
+      </c>
+      <c r="D15" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E15" t="n">
+        <v>23866.10812625995</v>
+      </c>
+      <c r="F15" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G15" t="n">
+        <v>35682.15048479443</v>
+      </c>
+      <c r="H15" t="n">
+        <v>6386.159649776772</v>
+      </c>
+      <c r="I15" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J15" t="n">
+        <v>6563.507414174516</v>
+      </c>
+      <c r="K15" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L15" t="n">
+        <v>12949.66706395129</v>
+      </c>
+      <c r="M15" t="n">
+        <v>14562.12832540515</v>
+      </c>
+      <c r="N15" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O15" t="n">
+        <v>28561.87171085741</v>
+      </c>
+      <c r="P15" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>43124.00003626257</v>
+      </c>
+      <c r="R15" t="n">
+        <v>9501.558353271153</v>
+      </c>
+      <c r="S15" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T15" t="n">
+        <v>11197.15648320555</v>
+      </c>
+      <c r="U15" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V15" t="n">
+        <v>20698.7148364767</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEMID03.csv</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SEMID03.csv</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>21196.15355487484</v>
+      </c>
+      <c r="D16" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E16" t="n">
+        <v>18738.12583115541</v>
+      </c>
+      <c r="F16" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G16" t="n">
+        <v>39934.27938603026</v>
+      </c>
+      <c r="H16" t="n">
+        <v>10588.43485062435</v>
+      </c>
+      <c r="I16" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J16" t="n">
+        <v>10895.89479396824</v>
+      </c>
+      <c r="K16" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L16" t="n">
+        <v>21484.32964459259</v>
+      </c>
+      <c r="M16" t="n">
+        <v>14200.6264220301</v>
+      </c>
+      <c r="N16" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O16" t="n">
+        <v>8554.430619060649</v>
+      </c>
+      <c r="P16" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>22755.05704109075</v>
+      </c>
+      <c r="R16" t="n">
+        <v>8705.923375734821</v>
+      </c>
+      <c r="S16" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T16" t="n">
+        <v>9513.835772774362</v>
+      </c>
+      <c r="U16" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V16" t="n">
+        <v>18219.75914850918</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEMID04.csv</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SEMID04.csv</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>4342.229776705455</v>
+      </c>
+      <c r="D17" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E17" t="n">
+        <v>14071.99994179747</v>
+      </c>
+      <c r="F17" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G17" t="n">
+        <v>18414.22971850293</v>
+      </c>
+      <c r="H17" t="n">
+        <v>4199.883421021588</v>
+      </c>
+      <c r="I17" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J17" t="n">
+        <v>4188.65218257867</v>
+      </c>
+      <c r="K17" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L17" t="n">
+        <v>8388.535603600259</v>
+      </c>
+      <c r="M17" t="n">
+        <v>20600.67860695353</v>
+      </c>
+      <c r="N17" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O17" t="n">
+        <v>16305.63978504031</v>
+      </c>
+      <c r="P17" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>36906.31839199384</v>
+      </c>
+      <c r="R17" t="n">
+        <v>8909.727794661751</v>
+      </c>
+      <c r="S17" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T17" t="n">
+        <v>8633.895387519586</v>
+      </c>
+      <c r="U17" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V17" t="n">
+        <v>17543.62318218133</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEMID05.csv</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SEMID05.csv</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>6062.726295363517</v>
+      </c>
+      <c r="D18" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3348.667392747715</v>
+      </c>
+      <c r="F18" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G18" t="n">
+        <v>9411.393688111231</v>
+      </c>
+      <c r="H18" t="n">
+        <v>4199.556268052334</v>
+      </c>
+      <c r="I18" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J18" t="n">
+        <v>4314.999640455026</v>
+      </c>
+      <c r="K18" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L18" t="n">
+        <v>8514.55590850736</v>
+      </c>
+      <c r="M18" t="n">
+        <v>2412.227768657749</v>
+      </c>
+      <c r="N18" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O18" t="n">
+        <v>3029.422949738972</v>
+      </c>
+      <c r="P18" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>5441.650718396722</v>
+      </c>
+      <c r="R18" t="n">
+        <v>3468.013839298519</v>
+      </c>
+      <c r="S18" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T18" t="n">
+        <v>3965.099291668188</v>
+      </c>
+      <c r="U18" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V18" t="n">
+        <v>7433.113130966707</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEMID06.csv</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SEMID06.csv</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>7979.447119020227</v>
+      </c>
+      <c r="D19" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E19" t="n">
+        <v>11931.91178669574</v>
+      </c>
+      <c r="F19" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G19" t="n">
+        <v>19911.35890571597</v>
+      </c>
+      <c r="H19" t="n">
+        <v>10184.76120821928</v>
+      </c>
+      <c r="I19" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J19" t="n">
+        <v>10370.0717622412</v>
+      </c>
+      <c r="K19" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L19" t="n">
+        <v>20554.83297046048</v>
+      </c>
+      <c r="M19" t="n">
+        <v>6891.489985044728</v>
+      </c>
+      <c r="N19" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O19" t="n">
+        <v>6753.982674823353</v>
+      </c>
+      <c r="P19" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>13645.47265986808</v>
+      </c>
+      <c r="R19" t="n">
+        <v>9147.846287553788</v>
+      </c>
+      <c r="S19" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T19" t="n">
+        <v>9652.983290404169</v>
+      </c>
+      <c r="U19" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V19" t="n">
+        <v>18800.82957795796</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEMID07.csv</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SEMID07.csv</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>4428.264000132051</v>
+      </c>
+      <c r="D20" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3894.940732710009</v>
+      </c>
+      <c r="F20" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G20" t="n">
+        <v>8323.204732842061</v>
+      </c>
+      <c r="H20" t="n">
+        <v>6145.462414799574</v>
+      </c>
+      <c r="I20" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J20" t="n">
+        <v>6268.249336951426</v>
+      </c>
+      <c r="K20" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L20" t="n">
+        <v>12413.711751751</v>
+      </c>
+      <c r="M20" t="n">
+        <v>7668.108235440171</v>
+      </c>
+      <c r="N20" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O20" t="n">
+        <v>6907.852358610848</v>
+      </c>
+      <c r="P20" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>14575.96059405102</v>
+      </c>
+      <c r="R20" t="n">
+        <v>5855.724037738828</v>
+      </c>
+      <c r="S20" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T20" t="n">
+        <v>5973.764700303661</v>
+      </c>
+      <c r="U20" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V20" t="n">
+        <v>11829.48873804249</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEMID08.csv</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SEMID08.csv</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>12007.55240070339</v>
+      </c>
+      <c r="D21" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E21" t="n">
+        <v>11863.39411313115</v>
+      </c>
+      <c r="F21" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G21" t="n">
+        <v>23870.94651383455</v>
+      </c>
+      <c r="H21" t="n">
+        <v>7692.580371680614</v>
+      </c>
+      <c r="I21" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J21" t="n">
+        <v>7820.098886066949</v>
+      </c>
+      <c r="K21" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L21" t="n">
+        <v>15512.67925774756</v>
+      </c>
+      <c r="M21" t="n">
+        <v>18552.01922287816</v>
+      </c>
+      <c r="N21" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O21" t="n">
+        <v>20415.75187043882</v>
+      </c>
+      <c r="P21" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>38967.77109331698</v>
+      </c>
+      <c r="R21" t="n">
+        <v>5469.436893548719</v>
+      </c>
+      <c r="S21" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T21" t="n">
+        <v>8563.169240123923</v>
+      </c>
+      <c r="U21" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V21" t="n">
+        <v>14032.60613367264</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEMID09.csv</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SEMID09.csv</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>14212.46177343845</v>
+      </c>
+      <c r="D22" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E22" t="n">
+        <v>13670.392670335</v>
+      </c>
+      <c r="F22" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G22" t="n">
+        <v>27882.85444377345</v>
+      </c>
+      <c r="H22" t="n">
+        <v>9176.844786185033</v>
+      </c>
+      <c r="I22" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J22" t="n">
+        <v>8981.060813628501</v>
+      </c>
+      <c r="K22" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L22" t="n">
+        <v>18157.90559981353</v>
+      </c>
+      <c r="M22" t="n">
+        <v>9995.999929385194</v>
+      </c>
+      <c r="N22" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O22" t="n">
+        <v>15585.19313181951</v>
+      </c>
+      <c r="P22" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>25581.1930612047</v>
+      </c>
+      <c r="R22" t="n">
+        <v>10300.02042684595</v>
+      </c>
+      <c r="S22" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T22" t="n">
+        <v>10778.8296462981</v>
+      </c>
+      <c r="U22" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V22" t="n">
+        <v>21078.85007314405</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEMID10.csv</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SEMID10.csv</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>6749.716115347595</v>
+      </c>
+      <c r="D23" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E23" t="n">
+        <v>4500.369418307673</v>
+      </c>
+      <c r="F23" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G23" t="n">
+        <v>11250.08553365527</v>
+      </c>
+      <c r="H23" t="n">
+        <v>8710.841238991059</v>
+      </c>
+      <c r="I23" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J23" t="n">
+        <v>8864.407616942848</v>
+      </c>
+      <c r="K23" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L23" t="n">
+        <v>17575.24885593391</v>
+      </c>
+      <c r="M23" t="n">
+        <v>1320.081204898359</v>
+      </c>
+      <c r="N23" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O23" t="n">
+        <v>1797.965445600042</v>
+      </c>
+      <c r="P23" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>3118.046650498401</v>
+      </c>
+      <c r="R23" t="n">
+        <v>4123.792083122488</v>
+      </c>
+      <c r="S23" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T23" t="n">
+        <v>4085.681008191244</v>
+      </c>
+      <c r="U23" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V23" t="n">
+        <v>8209.473091313732</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEMID11.csv</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>SEMID11.csv</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>6513.123008902011</v>
+      </c>
+      <c r="D24" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E24" t="n">
+        <v>8069.79697883513</v>
+      </c>
+      <c r="F24" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G24" t="n">
+        <v>14582.91998773714</v>
+      </c>
+      <c r="H24" t="n">
+        <v>5833.151206257251</v>
+      </c>
+      <c r="I24" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J24" t="n">
+        <v>5600.089550107393</v>
+      </c>
+      <c r="K24" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L24" t="n">
+        <v>11433.24075636464</v>
+      </c>
+      <c r="M24" t="n">
+        <v>7270.202877036855</v>
+      </c>
+      <c r="N24" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O24" t="n">
+        <v>4516.726748909594</v>
+      </c>
+      <c r="P24" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>11786.92962594645</v>
+      </c>
+      <c r="R24" t="n">
+        <v>5353.270758713806</v>
+      </c>
+      <c r="S24" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T24" t="n">
+        <v>5112.704684432971</v>
+      </c>
+      <c r="U24" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V24" t="n">
+        <v>10465.97544314678</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/SEMID12.csv</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>SEMID12.csv</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>43587.89554370419</v>
+      </c>
+      <c r="D25" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E25" t="n">
+        <v>28366.14021980655</v>
+      </c>
+      <c r="F25" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G25" t="n">
+        <v>71954.03576351074</v>
+      </c>
+      <c r="H25" t="n">
+        <v>11461.8347137468</v>
+      </c>
+      <c r="I25" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J25" t="n">
+        <v>12015.7326728004</v>
+      </c>
+      <c r="K25" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L25" t="n">
+        <v>23477.56738654721</v>
+      </c>
+      <c r="M25" t="n">
+        <v>9452.27121341354</v>
+      </c>
+      <c r="N25" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O25" t="n">
+        <v>13747.59280403808</v>
+      </c>
+      <c r="P25" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>23199.86401745162</v>
+      </c>
+      <c r="R25" t="n">
+        <v>7916.231241654648</v>
+      </c>
+      <c r="S25" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T25" t="n">
+        <v>7925.570705046808</v>
+      </c>
+      <c r="U25" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V25" t="n">
+        <v>15841.80194670146</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/STANDINGD01.csv</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>STANDINGD01.csv</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C26" t="n">
         <v>21176.21191864776</v>
       </c>
-      <c r="D4" t="n">
-        <v>17999</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="D26" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E26" t="n">
         <v>18263.69262989775</v>
       </c>
-      <c r="F4" t="n">
-        <v>17999</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="F26" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G26" t="n">
         <v>39439.90454854551</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H26" t="n">
         <v>15582.85548083792</v>
       </c>
-      <c r="I4" t="n">
-        <v>17999</v>
-      </c>
-      <c r="J4" t="n">
+      <c r="I26" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J26" t="n">
         <v>17012.96076622347</v>
       </c>
-      <c r="K4" t="n">
-        <v>17999</v>
-      </c>
-      <c r="L4" t="n">
+      <c r="K26" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L26" t="n">
         <v>32595.81624706139</v>
       </c>
-      <c r="M4" t="n">
+      <c r="M26" t="n">
         <v>23389.33042514446</v>
       </c>
-      <c r="N4" t="n">
-        <v>17999</v>
-      </c>
-      <c r="O4" t="n">
+      <c r="N26" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O26" t="n">
         <v>22248.21312258438</v>
       </c>
-      <c r="P4" t="n">
-        <v>17999</v>
-      </c>
-      <c r="Q4" t="n">
+      <c r="P26" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q26" t="n">
         <v>45637.54354772884</v>
       </c>
-      <c r="R4" t="n">
+      <c r="R26" t="n">
         <v>13910.02384810666</v>
       </c>
-      <c r="S4" t="n">
-        <v>17999</v>
-      </c>
-      <c r="T4" t="n">
+      <c r="S26" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T26" t="n">
         <v>13998.87502220762</v>
       </c>
-      <c r="U4" t="n">
-        <v>17999</v>
-      </c>
-      <c r="V4" t="n">
+      <c r="U26" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V26" t="n">
         <v>27908.89887031429</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/STANDINGD02.csv</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>STANDINGD02.csv</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>22098.58287533777</v>
+      </c>
+      <c r="D27" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E27" t="n">
+        <v>29864.32542875793</v>
+      </c>
+      <c r="F27" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G27" t="n">
+        <v>51962.9083040957</v>
+      </c>
+      <c r="H27" t="n">
+        <v>10980.90236126216</v>
+      </c>
+      <c r="I27" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J27" t="n">
+        <v>11177.50005785145</v>
+      </c>
+      <c r="K27" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L27" t="n">
+        <v>22158.40241911361</v>
+      </c>
+      <c r="M27" t="n">
+        <v>42488.81273021732</v>
+      </c>
+      <c r="N27" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O27" t="n">
+        <v>38534.47756867308</v>
+      </c>
+      <c r="P27" t="n">
+        <v>17946</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>81023.29029889041</v>
+      </c>
+      <c r="R27" t="n">
+        <v>12085.00291297552</v>
+      </c>
+      <c r="S27" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T27" t="n">
+        <v>13651.31333440797</v>
+      </c>
+      <c r="U27" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V27" t="n">
+        <v>25736.3162473835</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/STANDINGD03.csv</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>STANDINGD03.csv</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>32046.24882074015</v>
+      </c>
+      <c r="D28" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E28" t="n">
+        <v>33518.92507170494</v>
+      </c>
+      <c r="F28" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G28" t="n">
+        <v>65565.17389244509</v>
+      </c>
+      <c r="H28" t="n">
+        <v>13110.9742539263</v>
+      </c>
+      <c r="I28" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J28" t="n">
+        <v>13539.17027491347</v>
+      </c>
+      <c r="K28" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L28" t="n">
+        <v>26650.14452883977</v>
+      </c>
+      <c r="M28" t="n">
+        <v>19829.07161087118</v>
+      </c>
+      <c r="N28" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O28" t="n">
+        <v>13025.6128208122</v>
+      </c>
+      <c r="P28" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>32854.68443168338</v>
+      </c>
+      <c r="R28" t="n">
+        <v>12900.31367748345</v>
+      </c>
+      <c r="S28" t="n">
+        <v>17971</v>
+      </c>
+      <c r="T28" t="n">
+        <v>12615.59696802539</v>
+      </c>
+      <c r="U28" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V28" t="n">
+        <v>25515.91064550884</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/STANDINGD04.csv</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>STANDINGD04.csv</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>5460.328624351762</v>
+      </c>
+      <c r="D29" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E29" t="n">
+        <v>8352.321626430212</v>
+      </c>
+      <c r="F29" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G29" t="n">
+        <v>13812.65025078198</v>
+      </c>
+      <c r="H29" t="n">
+        <v>4366.188008627154</v>
+      </c>
+      <c r="I29" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J29" t="n">
+        <v>4380.630423423861</v>
+      </c>
+      <c r="K29" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L29" t="n">
+        <v>8746.818432051015</v>
+      </c>
+      <c r="M29" t="n">
+        <v>14521.8475955511</v>
+      </c>
+      <c r="N29" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O29" t="n">
+        <v>12192.48473619957</v>
+      </c>
+      <c r="P29" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>26714.33233175067</v>
+      </c>
+      <c r="R29" t="n">
+        <v>6122.590203308673</v>
+      </c>
+      <c r="S29" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T29" t="n">
+        <v>5881.216278049278</v>
+      </c>
+      <c r="U29" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V29" t="n">
+        <v>12003.80648135795</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/STANDINGD05.csv</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>STANDINGD05.csv</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>13648.87533617075</v>
+      </c>
+      <c r="D30" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E30" t="n">
+        <v>16275.61194992271</v>
+      </c>
+      <c r="F30" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G30" t="n">
+        <v>29924.48728609346</v>
+      </c>
+      <c r="H30" t="n">
+        <v>5613.261607837083</v>
+      </c>
+      <c r="I30" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J30" t="n">
+        <v>5953.537399016293</v>
+      </c>
+      <c r="K30" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L30" t="n">
+        <v>11566.79900685338</v>
+      </c>
+      <c r="M30" t="n">
+        <v>15812.41072474131</v>
+      </c>
+      <c r="N30" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O30" t="n">
+        <v>16346.50469773553</v>
+      </c>
+      <c r="P30" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>32158.91542247684</v>
+      </c>
+      <c r="R30" t="n">
+        <v>5446.38222817402</v>
+      </c>
+      <c r="S30" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T30" t="n">
+        <v>5485.863816937688</v>
+      </c>
+      <c r="U30" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V30" t="n">
+        <v>10932.24604511171</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/STANDINGD06.csv</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>STANDINGD06.csv</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>26821.49535914048</v>
+      </c>
+      <c r="D31" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E31" t="n">
+        <v>32803.11098034502</v>
+      </c>
+      <c r="F31" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G31" t="n">
+        <v>59624.6063394855</v>
+      </c>
+      <c r="H31" t="n">
+        <v>11834.04499776928</v>
+      </c>
+      <c r="I31" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J31" t="n">
+        <v>11293.94056026477</v>
+      </c>
+      <c r="K31" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L31" t="n">
+        <v>23127.98555803404</v>
+      </c>
+      <c r="M31" t="n">
+        <v>21574.52079690276</v>
+      </c>
+      <c r="N31" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O31" t="n">
+        <v>23153.91188483687</v>
+      </c>
+      <c r="P31" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>44728.43268173964</v>
+      </c>
+      <c r="R31" t="n">
+        <v>10003.64276204621</v>
+      </c>
+      <c r="S31" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T31" t="n">
+        <v>10270.3267150318</v>
+      </c>
+      <c r="U31" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V31" t="n">
+        <v>20273.969477078</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/STANDINGD07.csv</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>STANDINGD07.csv</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>16897.22534945201</v>
+      </c>
+      <c r="D32" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E32" t="n">
+        <v>14388.63952828069</v>
+      </c>
+      <c r="F32" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G32" t="n">
+        <v>31285.8648777327</v>
+      </c>
+      <c r="H32" t="n">
+        <v>8659.345344181565</v>
+      </c>
+      <c r="I32" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J32" t="n">
+        <v>8768.015157176647</v>
+      </c>
+      <c r="K32" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L32" t="n">
+        <v>17427.36050135821</v>
+      </c>
+      <c r="M32" t="n">
+        <v>19448.48894015003</v>
+      </c>
+      <c r="N32" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O32" t="n">
+        <v>21105.89808517281</v>
+      </c>
+      <c r="P32" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>40554.38702532284</v>
+      </c>
+      <c r="R32" t="n">
+        <v>8612.782805378058</v>
+      </c>
+      <c r="S32" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T32" t="n">
+        <v>7882.877869492724</v>
+      </c>
+      <c r="U32" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V32" t="n">
+        <v>16495.66067487078</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/STANDINGD08.csv</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>STANDINGD08.csv</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>18724.25016231008</v>
+      </c>
+      <c r="D33" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E33" t="n">
+        <v>23476.98789336455</v>
+      </c>
+      <c r="F33" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G33" t="n">
+        <v>42201.23805567463</v>
+      </c>
+      <c r="H33" t="n">
+        <v>12114.9484506761</v>
+      </c>
+      <c r="I33" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J33" t="n">
+        <v>11726.52855374982</v>
+      </c>
+      <c r="K33" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L33" t="n">
+        <v>23841.47700442592</v>
+      </c>
+      <c r="M33" t="n">
+        <v>29564.68477898434</v>
+      </c>
+      <c r="N33" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O33" t="n">
+        <v>30153.20922963634</v>
+      </c>
+      <c r="P33" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>59717.89400862069</v>
+      </c>
+      <c r="R33" t="n">
+        <v>10418.55660994765</v>
+      </c>
+      <c r="S33" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T33" t="n">
+        <v>9797.215685037321</v>
+      </c>
+      <c r="U33" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V33" t="n">
+        <v>20215.77229498497</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/STANDINGD09.csv</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>STANDINGD09.csv</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>25841.74367997559</v>
+      </c>
+      <c r="D34" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E34" t="n">
+        <v>35670.63850441634</v>
+      </c>
+      <c r="F34" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G34" t="n">
+        <v>61512.38218439193</v>
+      </c>
+      <c r="H34" t="n">
+        <v>9703.725798195293</v>
+      </c>
+      <c r="I34" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J34" t="n">
+        <v>9410.986231047966</v>
+      </c>
+      <c r="K34" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L34" t="n">
+        <v>19114.71202924326</v>
+      </c>
+      <c r="M34" t="n">
+        <v>9852.143941464916</v>
+      </c>
+      <c r="N34" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O34" t="n">
+        <v>14819.17201685188</v>
+      </c>
+      <c r="P34" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>24671.31595831679</v>
+      </c>
+      <c r="R34" t="n">
+        <v>8364.228640354757</v>
+      </c>
+      <c r="S34" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T34" t="n">
+        <v>9075.228801450528</v>
+      </c>
+      <c r="U34" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V34" t="n">
+        <v>17439.45744180529</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/STANDINGD10.csv</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>STANDINGD10.csv</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>5292.374516602941</v>
+      </c>
+      <c r="D35" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E35" t="n">
+        <v>4797.825792101934</v>
+      </c>
+      <c r="F35" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G35" t="n">
+        <v>10090.20030870488</v>
+      </c>
+      <c r="H35" t="n">
+        <v>5524.36775103484</v>
+      </c>
+      <c r="I35" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J35" t="n">
+        <v>5523.561484191154</v>
+      </c>
+      <c r="K35" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L35" t="n">
+        <v>11047.92923522599</v>
+      </c>
+      <c r="M35" t="n">
+        <v>3806.538455293809</v>
+      </c>
+      <c r="N35" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O35" t="n">
+        <v>3715.732723370683</v>
+      </c>
+      <c r="P35" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>7522.271178664492</v>
+      </c>
+      <c r="R35" t="n">
+        <v>5269.672604238872</v>
+      </c>
+      <c r="S35" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T35" t="n">
+        <v>5519.673734602378</v>
+      </c>
+      <c r="U35" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V35" t="n">
+        <v>10789.34633884125</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/STANDINGD11.csv</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>STANDINGD11.csv</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>24068.02729944732</v>
+      </c>
+      <c r="D36" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E36" t="n">
+        <v>21627.66780951043</v>
+      </c>
+      <c r="F36" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G36" t="n">
+        <v>45695.69510895775</v>
+      </c>
+      <c r="H36" t="n">
+        <v>8294.436877532169</v>
+      </c>
+      <c r="I36" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J36" t="n">
+        <v>8733.710134585446</v>
+      </c>
+      <c r="K36" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L36" t="n">
+        <v>17028.14701211762</v>
+      </c>
+      <c r="M36" t="n">
+        <v>10211.51972542701</v>
+      </c>
+      <c r="N36" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O36" t="n">
+        <v>8113.544468554327</v>
+      </c>
+      <c r="P36" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>18325.06419398133</v>
+      </c>
+      <c r="R36" t="n">
+        <v>5867.532781247931</v>
+      </c>
+      <c r="S36" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T36" t="n">
+        <v>5643.294168463446</v>
+      </c>
+      <c r="U36" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V36" t="n">
+        <v>11510.82694971138</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>/Users/matysprecloux/Desktop/Master IEAP/Code MOTTET/Defense /SYNCOGESTM2/data/raw/VICON_CSV/STANDINGD12.csv</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>STANDINGD12.csv</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>60994.26020101574</v>
+      </c>
+      <c r="D37" t="n">
+        <v>17999</v>
+      </c>
+      <c r="E37" t="n">
+        <v>63935.13445774127</v>
+      </c>
+      <c r="F37" t="n">
+        <v>17999</v>
+      </c>
+      <c r="G37" t="n">
+        <v>124929.394658757</v>
+      </c>
+      <c r="H37" t="n">
+        <v>14641.32659974894</v>
+      </c>
+      <c r="I37" t="n">
+        <v>17999</v>
+      </c>
+      <c r="J37" t="n">
+        <v>16018.39398046219</v>
+      </c>
+      <c r="K37" t="n">
+        <v>17999</v>
+      </c>
+      <c r="L37" t="n">
+        <v>30659.72058021113</v>
+      </c>
+      <c r="M37" t="n">
+        <v>14893.07515419563</v>
+      </c>
+      <c r="N37" t="n">
+        <v>17999</v>
+      </c>
+      <c r="O37" t="n">
+        <v>14976.92722885404</v>
+      </c>
+      <c r="P37" t="n">
+        <v>17999</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>29870.00238304968</v>
+      </c>
+      <c r="R37" t="n">
+        <v>8237.031007434252</v>
+      </c>
+      <c r="S37" t="n">
+        <v>17999</v>
+      </c>
+      <c r="T37" t="n">
+        <v>7781.600251462677</v>
+      </c>
+      <c r="U37" t="n">
+        <v>17999</v>
+      </c>
+      <c r="V37" t="n">
+        <v>16018.63125889693</v>
       </c>
     </row>
   </sheetData>

</xml_diff>